<commit_message>
added and integrated Emag_AccessApp, Emag_Search and Emag_GetDataFromSearchResults workflows
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>fwf.mentorship</t>
+  </si>
+  <si>
+    <t>EmagUrl</t>
+  </si>
+  <si>
+    <t>https://www.emag.ro/homepage</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -623,7 +629,14 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>